<commit_message>
Register Register updated to segregate different types of register
</commit_message>
<xml_diff>
--- a/Register Register.xlsx
+++ b/Register Register.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Dropbox\Personal Projects\Python\Signalling_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448D8E62-F91C-4117-AE95-2E6234292BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFACF313-541E-4910-8ADF-2AB096266589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="1125" windowWidth="22950" windowHeight="17400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1830" windowWidth="24420" windowHeight="17400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slave Addresses" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="173">
   <si>
     <t>Binary Inputs</t>
   </si>
@@ -521,6 +521,42 @@
   </si>
   <si>
     <t>Calibration averaging period</t>
+  </si>
+  <si>
+    <t>deprecated</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>Baud Rate</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1 = 19200, 2 = 57600, 3 = 115200</t>
+  </si>
+  <si>
+    <t>Board Type</t>
+  </si>
+  <si>
+    <t>2 = Axlecounter, 3 = Plunger Input, 4 = Signals, 5 = Points</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>generic settings</t>
+  </si>
+  <si>
+    <t>specific settings</t>
   </si>
 </sst>
 </file>
@@ -899,7 +935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F249"/>
   <sheetViews>
-    <sheetView topLeftCell="A214" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B250" sqref="B250"/>
     </sheetView>
   </sheetViews>
@@ -2531,10 +2567,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:G502"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E203" sqref="E203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2543,15 +2579,16 @@
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" customWidth="1"/>
+    <col min="5" max="5" width="126.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -2567,8 +2604,14 @@
       <c r="E2" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2579,13 +2622,16 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>165</v>
       </c>
       <c r="E3" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2601,8 +2647,11 @@
       <c r="E4" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2618,8 +2667,11 @@
       <c r="E5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2635,8 +2687,11 @@
       <c r="E6" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2652,8 +2707,11 @@
       <c r="E7" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2669,8 +2727,11 @@
       <c r="E8" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2686,8 +2747,11 @@
       <c r="E9" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2703,8 +2767,11 @@
       <c r="E10" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2720,8 +2787,11 @@
       <c r="E11" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2737,8 +2807,11 @@
       <c r="E12" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2754,8 +2827,14 @@
       <c r="E13" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>163</v>
+      </c>
+      <c r="G13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2771,8 +2850,14 @@
       <c r="E14" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>163</v>
+      </c>
+      <c r="G14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2788,8 +2873,14 @@
       <c r="E15" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2805,8 +2896,14 @@
       <c r="E16" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>163</v>
+      </c>
+      <c r="G16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2822,8 +2919,14 @@
       <c r="E17" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2839,8 +2942,11 @@
       <c r="E18" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2856,8 +2962,11 @@
       <c r="E19" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2873,8 +2982,11 @@
       <c r="E20" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2890,179 +3002,4118 @@
       <c r="E21" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>40020</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>40021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>40022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>40023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>40024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>40025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
+      <c r="B28">
+        <v>40026</v>
+      </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
+      <c r="B29">
+        <v>40027</v>
+      </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>40028</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>40029</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>40030</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>40031</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>40032</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>40033</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>40034</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>40035</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>40036</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>40037</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>40038</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>40039</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>40040</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>40041</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>40042</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>42</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>40043</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>40044</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>44</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>40045</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>45</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>40046</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>40047</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>40048</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>48</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>40049</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>49</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>40050</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
       <c r="B53">
         <v>40051</v>
       </c>
-      <c r="C53" t="s">
+    </row>
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54">
+        <v>40052</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55">
+        <v>40053</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <v>40054</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>54</v>
+      </c>
+      <c r="B57">
+        <v>40055</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <v>40056</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>56</v>
+      </c>
+      <c r="B59">
+        <v>40057</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>57</v>
+      </c>
+      <c r="B60">
+        <v>40058</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>58</v>
+      </c>
+      <c r="B61">
+        <v>40059</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>59</v>
+      </c>
+      <c r="B62">
+        <v>40060</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>60</v>
+      </c>
+      <c r="B63">
+        <v>40061</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>61</v>
+      </c>
+      <c r="B64">
+        <v>40062</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>62</v>
+      </c>
+      <c r="B65">
+        <v>40063</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>63</v>
+      </c>
+      <c r="B66">
+        <v>40064</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>64</v>
+      </c>
+      <c r="B67">
+        <v>40065</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>65</v>
+      </c>
+      <c r="B68">
+        <v>40066</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>66</v>
+      </c>
+      <c r="B69">
+        <v>40067</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>67</v>
+      </c>
+      <c r="B70">
+        <v>40068</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>68</v>
+      </c>
+      <c r="B71">
+        <v>40069</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>69</v>
+      </c>
+      <c r="B72">
+        <v>40070</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>70</v>
+      </c>
+      <c r="B73">
+        <v>40071</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>71</v>
+      </c>
+      <c r="B74">
+        <v>40072</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>72</v>
+      </c>
+      <c r="B75">
+        <v>40073</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>73</v>
+      </c>
+      <c r="B76">
+        <v>40074</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>74</v>
+      </c>
+      <c r="B77">
+        <v>40075</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>75</v>
+      </c>
+      <c r="B78">
+        <v>40076</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>76</v>
+      </c>
+      <c r="B79">
+        <v>40077</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>77</v>
+      </c>
+      <c r="B80">
+        <v>40078</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>78</v>
+      </c>
+      <c r="B81">
+        <v>40079</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>79</v>
+      </c>
+      <c r="B82">
+        <v>40080</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>80</v>
+      </c>
+      <c r="B83">
+        <v>40081</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>81</v>
+      </c>
+      <c r="B84">
+        <v>40082</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>82</v>
+      </c>
+      <c r="B85">
+        <v>40083</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>83</v>
+      </c>
+      <c r="B86">
+        <v>40084</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>84</v>
+      </c>
+      <c r="B87">
+        <v>40085</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>85</v>
+      </c>
+      <c r="B88">
+        <v>40086</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>86</v>
+      </c>
+      <c r="B89">
+        <v>40087</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>87</v>
+      </c>
+      <c r="B90">
+        <v>40088</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>88</v>
+      </c>
+      <c r="B91">
+        <v>40089</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>89</v>
+      </c>
+      <c r="B92">
+        <v>40090</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>90</v>
+      </c>
+      <c r="B93">
+        <v>40091</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>91</v>
+      </c>
+      <c r="B94">
+        <v>40092</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>92</v>
+      </c>
+      <c r="B95">
+        <v>40093</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>93</v>
+      </c>
+      <c r="B96">
+        <v>40094</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>94</v>
+      </c>
+      <c r="B97">
+        <v>40095</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>95</v>
+      </c>
+      <c r="B98">
+        <v>40096</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>96</v>
+      </c>
+      <c r="B99">
+        <v>40097</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>97</v>
+      </c>
+      <c r="B100">
+        <v>40098</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>98</v>
+      </c>
+      <c r="B101">
+        <v>40099</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>99</v>
+      </c>
+      <c r="B102">
+        <v>40100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>100</v>
+      </c>
+      <c r="B103">
+        <v>40101</v>
+      </c>
+      <c r="C103" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103" t="s">
+        <v>165</v>
+      </c>
+      <c r="E103" t="s">
+        <v>150</v>
+      </c>
+      <c r="F103" t="s">
+        <v>163</v>
+      </c>
+      <c r="G103" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>101</v>
+      </c>
+      <c r="B104">
+        <v>40102</v>
+      </c>
+      <c r="C104" t="s">
+        <v>164</v>
+      </c>
+      <c r="D104" t="s">
+        <v>165</v>
+      </c>
+      <c r="E104" t="s">
+        <v>166</v>
+      </c>
+      <c r="F104" t="s">
+        <v>163</v>
+      </c>
+      <c r="G104" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>102</v>
+      </c>
+      <c r="B105">
+        <v>40103</v>
+      </c>
+      <c r="C105" t="s">
+        <v>167</v>
+      </c>
+      <c r="D105" t="s">
+        <v>165</v>
+      </c>
+      <c r="E105" t="s">
+        <v>168</v>
+      </c>
+      <c r="F105" t="s">
+        <v>163</v>
+      </c>
+      <c r="G105" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>103</v>
+      </c>
+      <c r="B106">
+        <v>40104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>104</v>
+      </c>
+      <c r="B107">
+        <v>40105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>105</v>
+      </c>
+      <c r="B108">
+        <v>40106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>106</v>
+      </c>
+      <c r="B109">
+        <v>40107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>107</v>
+      </c>
+      <c r="B110">
+        <v>40108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>108</v>
+      </c>
+      <c r="B111">
+        <v>40109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>109</v>
+      </c>
+      <c r="B112">
+        <v>40110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>110</v>
+      </c>
+      <c r="B113">
+        <v>40111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>111</v>
+      </c>
+      <c r="B114">
+        <v>40112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A115">
         <v>112</v>
       </c>
-      <c r="D53" t="s">
+      <c r="B115">
+        <v>40113</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>113</v>
+      </c>
+      <c r="B116">
+        <v>40114</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>114</v>
+      </c>
+      <c r="B117">
+        <v>40115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>115</v>
+      </c>
+      <c r="B118">
+        <v>40116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>116</v>
+      </c>
+      <c r="B119">
+        <v>40117</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>117</v>
+      </c>
+      <c r="B120">
+        <v>40118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>118</v>
+      </c>
+      <c r="B121">
+        <v>40119</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>119</v>
+      </c>
+      <c r="B122">
+        <v>40120</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>120</v>
+      </c>
+      <c r="B123">
+        <v>40121</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>121</v>
+      </c>
+      <c r="B124">
+        <v>40122</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>122</v>
+      </c>
+      <c r="B125">
+        <v>40123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>123</v>
+      </c>
+      <c r="B126">
+        <v>40124</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>124</v>
+      </c>
+      <c r="B127">
+        <v>40125</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>125</v>
+      </c>
+      <c r="B128">
+        <v>40126</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>126</v>
+      </c>
+      <c r="B129">
+        <v>40127</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>127</v>
+      </c>
+      <c r="B130">
+        <v>40128</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>128</v>
+      </c>
+      <c r="B131">
+        <v>40129</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>129</v>
+      </c>
+      <c r="B132">
+        <v>40130</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>130</v>
+      </c>
+      <c r="B133">
+        <v>40131</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>131</v>
+      </c>
+      <c r="B134">
+        <v>40132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>132</v>
+      </c>
+      <c r="B135">
+        <v>40133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>133</v>
+      </c>
+      <c r="B136">
+        <v>40134</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>134</v>
+      </c>
+      <c r="B137">
+        <v>40135</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>135</v>
+      </c>
+      <c r="B138">
+        <v>40136</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>136</v>
+      </c>
+      <c r="B139">
+        <v>40137</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>137</v>
+      </c>
+      <c r="B140">
+        <v>40138</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>138</v>
+      </c>
+      <c r="B141">
+        <v>40139</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>139</v>
+      </c>
+      <c r="B142">
+        <v>40140</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>140</v>
+      </c>
+      <c r="B143">
+        <v>40141</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>141</v>
+      </c>
+      <c r="B144">
+        <v>40142</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>142</v>
+      </c>
+      <c r="B145">
+        <v>40143</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>143</v>
+      </c>
+      <c r="B146">
+        <v>40144</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>144</v>
+      </c>
+      <c r="B147">
+        <v>40145</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>145</v>
+      </c>
+      <c r="B148">
+        <v>40146</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>146</v>
+      </c>
+      <c r="B149">
+        <v>40147</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>147</v>
+      </c>
+      <c r="B150">
+        <v>40148</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>148</v>
+      </c>
+      <c r="B151">
+        <v>40149</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>149</v>
+      </c>
+      <c r="B152">
+        <v>40150</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>150</v>
+      </c>
+      <c r="B153">
+        <v>40151</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>151</v>
+      </c>
+      <c r="B154">
+        <v>40152</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>152</v>
+      </c>
+      <c r="B155">
+        <v>40153</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>153</v>
+      </c>
+      <c r="B156">
+        <v>40154</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>154</v>
+      </c>
+      <c r="B157">
+        <v>40155</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>155</v>
+      </c>
+      <c r="B158">
+        <v>40156</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>156</v>
+      </c>
+      <c r="B159">
+        <v>40157</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>157</v>
+      </c>
+      <c r="B160">
+        <v>40158</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>158</v>
+      </c>
+      <c r="B161">
+        <v>40159</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>159</v>
+      </c>
+      <c r="B162">
+        <v>40160</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>160</v>
+      </c>
+      <c r="B163">
+        <v>40161</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>161</v>
+      </c>
+      <c r="B164">
+        <v>40162</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>162</v>
+      </c>
+      <c r="B165">
+        <v>40163</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>163</v>
+      </c>
+      <c r="B166">
+        <v>40164</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>164</v>
+      </c>
+      <c r="B167">
+        <v>40165</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>165</v>
+      </c>
+      <c r="B168">
+        <v>40166</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>166</v>
+      </c>
+      <c r="B169">
+        <v>40167</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>167</v>
+      </c>
+      <c r="B170">
+        <v>40168</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>168</v>
+      </c>
+      <c r="B171">
+        <v>40169</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>169</v>
+      </c>
+      <c r="B172">
+        <v>40170</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>170</v>
+      </c>
+      <c r="B173">
+        <v>40171</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>171</v>
+      </c>
+      <c r="B174">
+        <v>40172</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>172</v>
+      </c>
+      <c r="B175">
+        <v>40173</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>173</v>
+      </c>
+      <c r="B176">
+        <v>40174</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>174</v>
+      </c>
+      <c r="B177">
+        <v>40175</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>175</v>
+      </c>
+      <c r="B178">
+        <v>40176</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>176</v>
+      </c>
+      <c r="B179">
+        <v>40177</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>177</v>
+      </c>
+      <c r="B180">
+        <v>40178</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>178</v>
+      </c>
+      <c r="B181">
+        <v>40179</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>179</v>
+      </c>
+      <c r="B182">
+        <v>40180</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>180</v>
+      </c>
+      <c r="B183">
+        <v>40181</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>181</v>
+      </c>
+      <c r="B184">
+        <v>40182</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>182</v>
+      </c>
+      <c r="B185">
+        <v>40183</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>183</v>
+      </c>
+      <c r="B186">
+        <v>40184</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>184</v>
+      </c>
+      <c r="B187">
+        <v>40185</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>185</v>
+      </c>
+      <c r="B188">
+        <v>40186</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>186</v>
+      </c>
+      <c r="B189">
+        <v>40187</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>187</v>
+      </c>
+      <c r="B190">
+        <v>40188</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>188</v>
+      </c>
+      <c r="B191">
+        <v>40189</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>189</v>
+      </c>
+      <c r="B192">
+        <v>40190</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>190</v>
+      </c>
+      <c r="B193">
+        <v>40191</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>191</v>
+      </c>
+      <c r="B194">
+        <v>40192</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>192</v>
+      </c>
+      <c r="B195">
+        <v>40193</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>193</v>
+      </c>
+      <c r="B196">
+        <v>40194</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>194</v>
+      </c>
+      <c r="B197">
+        <v>40195</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>195</v>
+      </c>
+      <c r="B198">
+        <v>40196</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>196</v>
+      </c>
+      <c r="B199">
+        <v>40197</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>197</v>
+      </c>
+      <c r="B200">
+        <v>40198</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>198</v>
+      </c>
+      <c r="B201">
+        <v>40199</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>199</v>
+      </c>
+      <c r="B202">
+        <v>40200</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>200</v>
+      </c>
+      <c r="B203">
+        <v>40201</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>201</v>
+      </c>
+      <c r="B204">
+        <v>40202</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D204" t="s">
+        <v>6</v>
+      </c>
+      <c r="E204" t="s">
+        <v>155</v>
+      </c>
+      <c r="F204" t="s">
+        <v>163</v>
+      </c>
+      <c r="G204" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>202</v>
+      </c>
+      <c r="B205">
+        <v>40203</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D205" t="s">
+        <v>6</v>
+      </c>
+      <c r="E205" t="s">
+        <v>155</v>
+      </c>
+      <c r="F205" t="s">
+        <v>163</v>
+      </c>
+      <c r="G205" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>203</v>
+      </c>
+      <c r="B206">
+        <v>40204</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D206" t="s">
+        <v>6</v>
+      </c>
+      <c r="E206" t="s">
+        <v>155</v>
+      </c>
+      <c r="F206" t="s">
+        <v>163</v>
+      </c>
+      <c r="G206" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>204</v>
+      </c>
+      <c r="B207">
+        <v>40205</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D207" t="s">
+        <v>6</v>
+      </c>
+      <c r="E207" t="s">
+        <v>156</v>
+      </c>
+      <c r="F207" t="s">
+        <v>163</v>
+      </c>
+      <c r="G207" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>205</v>
+      </c>
+      <c r="B208">
+        <v>40206</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D208" t="s">
+        <v>6</v>
+      </c>
+      <c r="E208" t="s">
+        <v>156</v>
+      </c>
+      <c r="F208" t="s">
+        <v>163</v>
+      </c>
+      <c r="G208" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>206</v>
+      </c>
+      <c r="B209">
+        <v>40207</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D209" t="s">
+        <v>6</v>
+      </c>
+      <c r="E209" t="s">
+        <v>156</v>
+      </c>
+      <c r="F209" t="s">
+        <v>163</v>
+      </c>
+      <c r="G209" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>207</v>
+      </c>
+      <c r="B210">
+        <v>40208</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D210" t="s">
+        <v>6</v>
+      </c>
+      <c r="E210" t="s">
+        <v>157</v>
+      </c>
+      <c r="F210" t="s">
+        <v>163</v>
+      </c>
+      <c r="G210" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>208</v>
+      </c>
+      <c r="B211">
+        <v>40209</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D211" t="s">
+        <v>6</v>
+      </c>
+      <c r="E211" t="s">
+        <v>157</v>
+      </c>
+      <c r="F211" t="s">
+        <v>163</v>
+      </c>
+      <c r="G211" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>209</v>
+      </c>
+      <c r="B212">
+        <v>40210</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D212" t="s">
+        <v>6</v>
+      </c>
+      <c r="E212" t="s">
+        <v>157</v>
+      </c>
+      <c r="F212" t="s">
+        <v>163</v>
+      </c>
+      <c r="G212" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>210</v>
+      </c>
+      <c r="B213">
+        <v>40211</v>
+      </c>
+      <c r="C213" s="1"/>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>211</v>
+      </c>
+      <c r="B214">
+        <v>40212</v>
+      </c>
+      <c r="C214" s="1"/>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>212</v>
+      </c>
+      <c r="B215">
+        <v>40213</v>
+      </c>
+      <c r="C215" s="1"/>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>213</v>
+      </c>
+      <c r="B216">
+        <v>40214</v>
+      </c>
+      <c r="C216" s="1"/>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>214</v>
+      </c>
+      <c r="B217">
+        <v>40215</v>
+      </c>
+      <c r="C217" s="1"/>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>215</v>
+      </c>
+      <c r="B218">
+        <v>40216</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D218" t="s">
+        <v>6</v>
+      </c>
+      <c r="E218" t="s">
+        <v>159</v>
+      </c>
+      <c r="F218" t="s">
+        <v>163</v>
+      </c>
+      <c r="G218" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>216</v>
+      </c>
+      <c r="B219">
+        <v>40217</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D219" t="s">
+        <v>6</v>
+      </c>
+      <c r="E219" t="s">
+        <v>159</v>
+      </c>
+      <c r="F219" t="s">
+        <v>163</v>
+      </c>
+      <c r="G219" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>217</v>
+      </c>
+      <c r="B220">
+        <v>40218</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D220" t="s">
+        <v>6</v>
+      </c>
+      <c r="E220" t="s">
+        <v>159</v>
+      </c>
+      <c r="F220" t="s">
+        <v>163</v>
+      </c>
+      <c r="G220" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>218</v>
+      </c>
+      <c r="B221">
+        <v>40219</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D221" t="s">
+        <v>6</v>
+      </c>
+      <c r="E221" t="s">
+        <v>153</v>
+      </c>
+      <c r="F221" t="s">
+        <v>163</v>
+      </c>
+      <c r="G221" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>219</v>
+      </c>
+      <c r="B222">
+        <v>40220</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>220</v>
+      </c>
+      <c r="B223">
+        <v>40221</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>221</v>
+      </c>
+      <c r="B224">
+        <v>40222</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>222</v>
+      </c>
+      <c r="B225">
+        <v>40223</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>223</v>
+      </c>
+      <c r="B226">
+        <v>40224</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>224</v>
+      </c>
+      <c r="B227">
+        <v>40225</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>225</v>
+      </c>
+      <c r="B228">
+        <v>40226</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>226</v>
+      </c>
+      <c r="B229">
+        <v>40227</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>227</v>
+      </c>
+      <c r="B230">
+        <v>40228</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>228</v>
+      </c>
+      <c r="B231">
+        <v>40229</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>229</v>
+      </c>
+      <c r="B232">
+        <v>40230</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>230</v>
+      </c>
+      <c r="B233">
+        <v>40231</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>231</v>
+      </c>
+      <c r="B234">
+        <v>40232</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>232</v>
+      </c>
+      <c r="B235">
+        <v>40233</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>233</v>
+      </c>
+      <c r="B236">
+        <v>40234</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>234</v>
+      </c>
+      <c r="B237">
+        <v>40235</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>235</v>
+      </c>
+      <c r="B238">
+        <v>40236</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>236</v>
+      </c>
+      <c r="B239">
+        <v>40237</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>237</v>
+      </c>
+      <c r="B240">
+        <v>40238</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>238</v>
+      </c>
+      <c r="B241">
+        <v>40239</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>239</v>
+      </c>
+      <c r="B242">
+        <v>40240</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>240</v>
+      </c>
+      <c r="B243">
+        <v>40241</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>241</v>
+      </c>
+      <c r="B244">
+        <v>40242</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>242</v>
+      </c>
+      <c r="B245">
+        <v>40243</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>243</v>
+      </c>
+      <c r="B246">
+        <v>40244</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>244</v>
+      </c>
+      <c r="B247">
+        <v>40245</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>245</v>
+      </c>
+      <c r="B248">
+        <v>40246</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>246</v>
+      </c>
+      <c r="B249">
+        <v>40247</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>247</v>
+      </c>
+      <c r="B250">
+        <v>40248</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>248</v>
+      </c>
+      <c r="B251">
+        <v>40249</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>249</v>
+      </c>
+      <c r="B252">
+        <v>40250</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>250</v>
+      </c>
+      <c r="B253">
+        <v>40251</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>251</v>
+      </c>
+      <c r="B254">
+        <v>40252</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>252</v>
+      </c>
+      <c r="B255">
+        <v>40253</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>253</v>
+      </c>
+      <c r="B256">
+        <v>40254</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>254</v>
+      </c>
+      <c r="B257">
+        <v>40255</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>255</v>
+      </c>
+      <c r="B258">
+        <v>40256</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>256</v>
+      </c>
+      <c r="B259">
+        <v>40257</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>257</v>
+      </c>
+      <c r="B260">
+        <v>40258</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>258</v>
+      </c>
+      <c r="B261">
+        <v>40259</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>259</v>
+      </c>
+      <c r="B262">
+        <v>40260</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>260</v>
+      </c>
+      <c r="B263">
+        <v>40261</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>261</v>
+      </c>
+      <c r="B264">
+        <v>40262</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>262</v>
+      </c>
+      <c r="B265">
+        <v>40263</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>263</v>
+      </c>
+      <c r="B266">
+        <v>40264</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>264</v>
+      </c>
+      <c r="B267">
+        <v>40265</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>265</v>
+      </c>
+      <c r="B268">
+        <v>40266</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>266</v>
+      </c>
+      <c r="B269">
+        <v>40267</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>267</v>
+      </c>
+      <c r="B270">
+        <v>40268</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>268</v>
+      </c>
+      <c r="B271">
+        <v>40269</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>269</v>
+      </c>
+      <c r="B272">
+        <v>40270</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>270</v>
+      </c>
+      <c r="B273">
+        <v>40271</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>271</v>
+      </c>
+      <c r="B274">
+        <v>40272</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>272</v>
+      </c>
+      <c r="B275">
+        <v>40273</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>273</v>
+      </c>
+      <c r="B276">
+        <v>40274</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>274</v>
+      </c>
+      <c r="B277">
+        <v>40275</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>275</v>
+      </c>
+      <c r="B278">
+        <v>40276</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>276</v>
+      </c>
+      <c r="B279">
+        <v>40277</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>277</v>
+      </c>
+      <c r="B280">
+        <v>40278</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>278</v>
+      </c>
+      <c r="B281">
+        <v>40279</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>279</v>
+      </c>
+      <c r="B282">
+        <v>40280</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>280</v>
+      </c>
+      <c r="B283">
+        <v>40281</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>281</v>
+      </c>
+      <c r="B284">
+        <v>40282</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>282</v>
+      </c>
+      <c r="B285">
+        <v>40283</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>283</v>
+      </c>
+      <c r="B286">
+        <v>40284</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>284</v>
+      </c>
+      <c r="B287">
+        <v>40285</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>285</v>
+      </c>
+      <c r="B288">
+        <v>40286</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>286</v>
+      </c>
+      <c r="B289">
+        <v>40287</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>287</v>
+      </c>
+      <c r="B290">
+        <v>40288</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>288</v>
+      </c>
+      <c r="B291">
+        <v>40289</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>289</v>
+      </c>
+      <c r="B292">
+        <v>40290</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>290</v>
+      </c>
+      <c r="B293">
+        <v>40291</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>291</v>
+      </c>
+      <c r="B294">
+        <v>40292</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>292</v>
+      </c>
+      <c r="B295">
+        <v>40293</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>293</v>
+      </c>
+      <c r="B296">
+        <v>40294</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>294</v>
+      </c>
+      <c r="B297">
+        <v>40295</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>295</v>
+      </c>
+      <c r="B298">
+        <v>40296</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>296</v>
+      </c>
+      <c r="B299">
+        <v>40297</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>297</v>
+      </c>
+      <c r="B300">
+        <v>40298</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>298</v>
+      </c>
+      <c r="B301">
+        <v>40299</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>299</v>
+      </c>
+      <c r="B302">
+        <v>40300</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>300</v>
+      </c>
+      <c r="B303">
+        <v>40301</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>301</v>
+      </c>
+      <c r="B304">
+        <v>40302</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>302</v>
+      </c>
+      <c r="B305">
+        <v>40303</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>303</v>
+      </c>
+      <c r="B306">
+        <v>40304</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>304</v>
+      </c>
+      <c r="B307">
+        <v>40305</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>305</v>
+      </c>
+      <c r="B308">
+        <v>40306</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>306</v>
+      </c>
+      <c r="B309">
+        <v>40307</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>307</v>
+      </c>
+      <c r="B310">
+        <v>40308</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>308</v>
+      </c>
+      <c r="B311">
+        <v>40309</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>309</v>
+      </c>
+      <c r="B312">
+        <v>40310</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>310</v>
+      </c>
+      <c r="B313">
+        <v>40311</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>311</v>
+      </c>
+      <c r="B314">
+        <v>40312</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>312</v>
+      </c>
+      <c r="B315">
+        <v>40313</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>313</v>
+      </c>
+      <c r="B316">
+        <v>40314</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>314</v>
+      </c>
+      <c r="B317">
+        <v>40315</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>315</v>
+      </c>
+      <c r="B318">
+        <v>40316</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>316</v>
+      </c>
+      <c r="B319">
+        <v>40317</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>317</v>
+      </c>
+      <c r="B320">
+        <v>40318</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>318</v>
+      </c>
+      <c r="B321">
+        <v>40319</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>319</v>
+      </c>
+      <c r="B322">
+        <v>40320</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>320</v>
+      </c>
+      <c r="B323">
+        <v>40321</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>321</v>
+      </c>
+      <c r="B324">
+        <v>40322</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>322</v>
+      </c>
+      <c r="B325">
+        <v>40323</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>323</v>
+      </c>
+      <c r="B326">
+        <v>40324</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>324</v>
+      </c>
+      <c r="B327">
+        <v>40325</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>325</v>
+      </c>
+      <c r="B328">
+        <v>40326</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>326</v>
+      </c>
+      <c r="B329">
+        <v>40327</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>327</v>
+      </c>
+      <c r="B330">
+        <v>40328</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>328</v>
+      </c>
+      <c r="B331">
+        <v>40329</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>329</v>
+      </c>
+      <c r="B332">
+        <v>40330</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>330</v>
+      </c>
+      <c r="B333">
+        <v>40331</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>331</v>
+      </c>
+      <c r="B334">
+        <v>40332</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>332</v>
+      </c>
+      <c r="B335">
+        <v>40333</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>333</v>
+      </c>
+      <c r="B336">
+        <v>40334</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>334</v>
+      </c>
+      <c r="B337">
+        <v>40335</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>335</v>
+      </c>
+      <c r="B338">
+        <v>40336</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>336</v>
+      </c>
+      <c r="B339">
+        <v>40337</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>337</v>
+      </c>
+      <c r="B340">
+        <v>40338</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>338</v>
+      </c>
+      <c r="B341">
+        <v>40339</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>339</v>
+      </c>
+      <c r="B342">
+        <v>40340</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>340</v>
+      </c>
+      <c r="B343">
+        <v>40341</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>341</v>
+      </c>
+      <c r="B344">
+        <v>40342</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>342</v>
+      </c>
+      <c r="B345">
+        <v>40343</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>343</v>
+      </c>
+      <c r="B346">
+        <v>40344</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>344</v>
+      </c>
+      <c r="B347">
+        <v>40345</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>345</v>
+      </c>
+      <c r="B348">
+        <v>40346</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>346</v>
+      </c>
+      <c r="B349">
+        <v>40347</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>347</v>
+      </c>
+      <c r="B350">
+        <v>40348</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>348</v>
+      </c>
+      <c r="B351">
+        <v>40349</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>349</v>
+      </c>
+      <c r="B352">
+        <v>40350</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>350</v>
+      </c>
+      <c r="B353">
+        <v>40351</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>351</v>
+      </c>
+      <c r="B354">
+        <v>40352</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>352</v>
+      </c>
+      <c r="B355">
+        <v>40353</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>353</v>
+      </c>
+      <c r="B356">
+        <v>40354</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>354</v>
+      </c>
+      <c r="B357">
+        <v>40355</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>355</v>
+      </c>
+      <c r="B358">
+        <v>40356</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>356</v>
+      </c>
+      <c r="B359">
+        <v>40357</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>357</v>
+      </c>
+      <c r="B360">
+        <v>40358</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>358</v>
+      </c>
+      <c r="B361">
+        <v>40359</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>359</v>
+      </c>
+      <c r="B362">
+        <v>40360</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>360</v>
+      </c>
+      <c r="B363">
+        <v>40361</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>361</v>
+      </c>
+      <c r="B364">
+        <v>40362</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>362</v>
+      </c>
+      <c r="B365">
+        <v>40363</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>363</v>
+      </c>
+      <c r="B366">
+        <v>40364</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>364</v>
+      </c>
+      <c r="B367">
+        <v>40365</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>365</v>
+      </c>
+      <c r="B368">
+        <v>40366</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>366</v>
+      </c>
+      <c r="B369">
+        <v>40367</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>367</v>
+      </c>
+      <c r="B370">
+        <v>40368</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>368</v>
+      </c>
+      <c r="B371">
+        <v>40369</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>369</v>
+      </c>
+      <c r="B372">
+        <v>40370</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A373">
+        <v>370</v>
+      </c>
+      <c r="B373">
+        <v>40371</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A374">
+        <v>371</v>
+      </c>
+      <c r="B374">
+        <v>40372</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A375">
+        <v>372</v>
+      </c>
+      <c r="B375">
+        <v>40373</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>373</v>
+      </c>
+      <c r="B376">
+        <v>40374</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>374</v>
+      </c>
+      <c r="B377">
+        <v>40375</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>375</v>
+      </c>
+      <c r="B378">
+        <v>40376</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>376</v>
+      </c>
+      <c r="B379">
+        <v>40377</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>377</v>
+      </c>
+      <c r="B380">
+        <v>40378</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>378</v>
+      </c>
+      <c r="B381">
+        <v>40379</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>379</v>
+      </c>
+      <c r="B382">
+        <v>40380</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>380</v>
+      </c>
+      <c r="B383">
+        <v>40381</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>381</v>
+      </c>
+      <c r="B384">
+        <v>40382</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>382</v>
+      </c>
+      <c r="B385">
+        <v>40383</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>383</v>
+      </c>
+      <c r="B386">
+        <v>40384</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>384</v>
+      </c>
+      <c r="B387">
+        <v>40385</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>385</v>
+      </c>
+      <c r="B388">
+        <v>40386</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>386</v>
+      </c>
+      <c r="B389">
+        <v>40387</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>387</v>
+      </c>
+      <c r="B390">
+        <v>40388</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>388</v>
+      </c>
+      <c r="B391">
+        <v>40389</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>389</v>
+      </c>
+      <c r="B392">
+        <v>40390</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>390</v>
+      </c>
+      <c r="B393">
+        <v>40391</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>391</v>
+      </c>
+      <c r="B394">
+        <v>40392</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>392</v>
+      </c>
+      <c r="B395">
+        <v>40393</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>393</v>
+      </c>
+      <c r="B396">
+        <v>40394</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>394</v>
+      </c>
+      <c r="B397">
+        <v>40395</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>395</v>
+      </c>
+      <c r="B398">
+        <v>40396</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>396</v>
+      </c>
+      <c r="B399">
+        <v>40397</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>397</v>
+      </c>
+      <c r="B400">
+        <v>40398</v>
+      </c>
+    </row>
+    <row r="401" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>398</v>
+      </c>
+      <c r="B401">
+        <v>40399</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>399</v>
+      </c>
+      <c r="B402">
+        <v>40400</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>400</v>
+      </c>
+      <c r="B403">
+        <v>40401</v>
+      </c>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>401</v>
+      </c>
+      <c r="B404">
+        <v>40402</v>
+      </c>
+      <c r="C404" t="s">
+        <v>112</v>
+      </c>
+      <c r="D404" t="s">
         <v>68</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E404" t="s">
         <v>113</v>
+      </c>
+      <c r="F404" t="s">
+        <v>163</v>
+      </c>
+      <c r="G404" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>402</v>
+      </c>
+      <c r="B405">
+        <v>40403</v>
+      </c>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>403</v>
+      </c>
+      <c r="B406">
+        <v>40404</v>
+      </c>
+    </row>
+    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>404</v>
+      </c>
+      <c r="B407">
+        <v>40405</v>
+      </c>
+    </row>
+    <row r="408" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>405</v>
+      </c>
+      <c r="B408">
+        <v>40406</v>
+      </c>
+    </row>
+    <row r="409" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>406</v>
+      </c>
+      <c r="B409">
+        <v>40407</v>
+      </c>
+    </row>
+    <row r="410" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A410">
+        <v>407</v>
+      </c>
+      <c r="B410">
+        <v>40408</v>
+      </c>
+    </row>
+    <row r="411" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A411">
+        <v>408</v>
+      </c>
+      <c r="B411">
+        <v>40409</v>
+      </c>
+    </row>
+    <row r="412" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A412">
+        <v>409</v>
+      </c>
+      <c r="B412">
+        <v>40410</v>
+      </c>
+    </row>
+    <row r="413" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A413">
+        <v>410</v>
+      </c>
+      <c r="B413">
+        <v>40411</v>
+      </c>
+    </row>
+    <row r="414" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A414">
+        <v>411</v>
+      </c>
+      <c r="B414">
+        <v>40412</v>
+      </c>
+    </row>
+    <row r="415" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A415">
+        <v>412</v>
+      </c>
+      <c r="B415">
+        <v>40413</v>
+      </c>
+    </row>
+    <row r="416" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A416">
+        <v>413</v>
+      </c>
+      <c r="B416">
+        <v>40414</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A417">
+        <v>414</v>
+      </c>
+      <c r="B417">
+        <v>40415</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A418">
+        <v>415</v>
+      </c>
+      <c r="B418">
+        <v>40416</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A419">
+        <v>416</v>
+      </c>
+      <c r="B419">
+        <v>40417</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A420">
+        <v>417</v>
+      </c>
+      <c r="B420">
+        <v>40418</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A421">
+        <v>418</v>
+      </c>
+      <c r="B421">
+        <v>40419</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A422">
+        <v>419</v>
+      </c>
+      <c r="B422">
+        <v>40420</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A423">
+        <v>420</v>
+      </c>
+      <c r="B423">
+        <v>40421</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A424">
+        <v>421</v>
+      </c>
+      <c r="B424">
+        <v>40422</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A425">
+        <v>422</v>
+      </c>
+      <c r="B425">
+        <v>40423</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A426">
+        <v>423</v>
+      </c>
+      <c r="B426">
+        <v>40424</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A427">
+        <v>424</v>
+      </c>
+      <c r="B427">
+        <v>40425</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A428">
+        <v>425</v>
+      </c>
+      <c r="B428">
+        <v>40426</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A429">
+        <v>426</v>
+      </c>
+      <c r="B429">
+        <v>40427</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A430">
+        <v>427</v>
+      </c>
+      <c r="B430">
+        <v>40428</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A431">
+        <v>428</v>
+      </c>
+      <c r="B431">
+        <v>40429</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432">
+        <v>429</v>
+      </c>
+      <c r="B432">
+        <v>40430</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A433">
+        <v>430</v>
+      </c>
+      <c r="B433">
+        <v>40431</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A434">
+        <v>431</v>
+      </c>
+      <c r="B434">
+        <v>40432</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A435">
+        <v>432</v>
+      </c>
+      <c r="B435">
+        <v>40433</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A436">
+        <v>433</v>
+      </c>
+      <c r="B436">
+        <v>40434</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A437">
+        <v>434</v>
+      </c>
+      <c r="B437">
+        <v>40435</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A438">
+        <v>435</v>
+      </c>
+      <c r="B438">
+        <v>40436</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A439">
+        <v>436</v>
+      </c>
+      <c r="B439">
+        <v>40437</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A440">
+        <v>437</v>
+      </c>
+      <c r="B440">
+        <v>40438</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A441">
+        <v>438</v>
+      </c>
+      <c r="B441">
+        <v>40439</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A442">
+        <v>439</v>
+      </c>
+      <c r="B442">
+        <v>40440</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A443">
+        <v>440</v>
+      </c>
+      <c r="B443">
+        <v>40441</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A444">
+        <v>441</v>
+      </c>
+      <c r="B444">
+        <v>40442</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A445">
+        <v>442</v>
+      </c>
+      <c r="B445">
+        <v>40443</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A446">
+        <v>443</v>
+      </c>
+      <c r="B446">
+        <v>40444</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A447">
+        <v>444</v>
+      </c>
+      <c r="B447">
+        <v>40445</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A448">
+        <v>445</v>
+      </c>
+      <c r="B448">
+        <v>40446</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>446</v>
+      </c>
+      <c r="B449">
+        <v>40447</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A450">
+        <v>447</v>
+      </c>
+      <c r="B450">
+        <v>40448</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A451">
+        <v>448</v>
+      </c>
+      <c r="B451">
+        <v>40449</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A452">
+        <v>449</v>
+      </c>
+      <c r="B452">
+        <v>40450</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A453">
+        <v>450</v>
+      </c>
+      <c r="B453">
+        <v>40451</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A454">
+        <v>451</v>
+      </c>
+      <c r="B454">
+        <v>40452</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A455">
+        <v>452</v>
+      </c>
+      <c r="B455">
+        <v>40453</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A456">
+        <v>453</v>
+      </c>
+      <c r="B456">
+        <v>40454</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A457">
+        <v>454</v>
+      </c>
+      <c r="B457">
+        <v>40455</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A458">
+        <v>455</v>
+      </c>
+      <c r="B458">
+        <v>40456</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A459">
+        <v>456</v>
+      </c>
+      <c r="B459">
+        <v>40457</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A460">
+        <v>457</v>
+      </c>
+      <c r="B460">
+        <v>40458</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A461">
+        <v>458</v>
+      </c>
+      <c r="B461">
+        <v>40459</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A462">
+        <v>459</v>
+      </c>
+      <c r="B462">
+        <v>40460</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A463">
+        <v>460</v>
+      </c>
+      <c r="B463">
+        <v>40461</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A464">
+        <v>461</v>
+      </c>
+      <c r="B464">
+        <v>40462</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A465">
+        <v>462</v>
+      </c>
+      <c r="B465">
+        <v>40463</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A466">
+        <v>463</v>
+      </c>
+      <c r="B466">
+        <v>40464</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A467">
+        <v>464</v>
+      </c>
+      <c r="B467">
+        <v>40465</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A468">
+        <v>465</v>
+      </c>
+      <c r="B468">
+        <v>40466</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A469">
+        <v>466</v>
+      </c>
+      <c r="B469">
+        <v>40467</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A470">
+        <v>467</v>
+      </c>
+      <c r="B470">
+        <v>40468</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A471">
+        <v>468</v>
+      </c>
+      <c r="B471">
+        <v>40469</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A472">
+        <v>469</v>
+      </c>
+      <c r="B472">
+        <v>40470</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A473">
+        <v>470</v>
+      </c>
+      <c r="B473">
+        <v>40471</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A474">
+        <v>471</v>
+      </c>
+      <c r="B474">
+        <v>40472</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A475">
+        <v>472</v>
+      </c>
+      <c r="B475">
+        <v>40473</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A476">
+        <v>473</v>
+      </c>
+      <c r="B476">
+        <v>40474</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A477">
+        <v>474</v>
+      </c>
+      <c r="B477">
+        <v>40475</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A478">
+        <v>475</v>
+      </c>
+      <c r="B478">
+        <v>40476</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A479">
+        <v>476</v>
+      </c>
+      <c r="B479">
+        <v>40477</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A480">
+        <v>477</v>
+      </c>
+      <c r="B480">
+        <v>40478</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A481">
+        <v>478</v>
+      </c>
+      <c r="B481">
+        <v>40479</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A482">
+        <v>479</v>
+      </c>
+      <c r="B482">
+        <v>40480</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A483">
+        <v>480</v>
+      </c>
+      <c r="B483">
+        <v>40481</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A484">
+        <v>481</v>
+      </c>
+      <c r="B484">
+        <v>40482</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A485">
+        <v>482</v>
+      </c>
+      <c r="B485">
+        <v>40483</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A486">
+        <v>483</v>
+      </c>
+      <c r="B486">
+        <v>40484</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A487">
+        <v>484</v>
+      </c>
+      <c r="B487">
+        <v>40485</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A488">
+        <v>485</v>
+      </c>
+      <c r="B488">
+        <v>40486</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A489">
+        <v>486</v>
+      </c>
+      <c r="B489">
+        <v>40487</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A490">
+        <v>487</v>
+      </c>
+      <c r="B490">
+        <v>40488</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A491">
+        <v>488</v>
+      </c>
+      <c r="B491">
+        <v>40489</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A492">
+        <v>489</v>
+      </c>
+      <c r="B492">
+        <v>40490</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A493">
+        <v>490</v>
+      </c>
+      <c r="B493">
+        <v>40491</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A494">
+        <v>491</v>
+      </c>
+      <c r="B494">
+        <v>40492</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A495">
+        <v>492</v>
+      </c>
+      <c r="B495">
+        <v>40493</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A496">
+        <v>493</v>
+      </c>
+      <c r="B496">
+        <v>40494</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A497">
+        <v>494</v>
+      </c>
+      <c r="B497">
+        <v>40495</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A498">
+        <v>495</v>
+      </c>
+      <c r="B498">
+        <v>40496</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A499">
+        <v>496</v>
+      </c>
+      <c r="B499">
+        <v>40497</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A500">
+        <v>497</v>
+      </c>
+      <c r="B500">
+        <v>40498</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A501">
+        <v>498</v>
+      </c>
+      <c r="B501">
+        <v>40499</v>
+      </c>
+    </row>
+    <row r="502" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A502">
+        <v>499</v>
+      </c>
+      <c r="B502">
+        <v>40500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Track Circuits Added Web Interface Editor Working Fixed Point Detection False issue
</commit_message>
<xml_diff>
--- a/Register Register.xlsx
+++ b/Register Register.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Dropbox\Personal Projects\Python\Signalling_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CABB307-DAF8-428E-A7EA-D7140ECD86F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F2F5DD-5CC4-4C13-9010-3F4821E78FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26715" yWindow="3075" windowWidth="24420" windowHeight="17085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17700" yWindow="2550" windowWidth="24420" windowHeight="17085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slave Addresses" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="185">
   <si>
     <t>Binary Inputs</t>
   </si>
@@ -575,6 +575,24 @@
   </si>
   <si>
     <t>Signal Box</t>
+  </si>
+  <si>
+    <t>Signal 1 - Level Crossing</t>
+  </si>
+  <si>
+    <t>50 Points</t>
+  </si>
+  <si>
+    <t>109 Signal</t>
+  </si>
+  <si>
+    <t>103 Signal</t>
+  </si>
+  <si>
+    <t>105 Signal</t>
+  </si>
+  <si>
+    <t>107 Signal</t>
   </si>
 </sst>
 </file>
@@ -953,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,11 +1663,23 @@
       <c r="A66" s="5">
         <v>64</v>
       </c>
+      <c r="B66" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>65</v>
       </c>
+      <c r="B67" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
@@ -1858,6 +1888,12 @@
       <c r="A105" s="5">
         <v>103</v>
       </c>
+      <c r="B105" t="s">
+        <v>25</v>
+      </c>
+      <c r="C105" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
@@ -1868,6 +1904,12 @@
       <c r="A107" s="5">
         <v>105</v>
       </c>
+      <c r="B107" t="s">
+        <v>25</v>
+      </c>
+      <c r="C107" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
@@ -1878,6 +1920,12 @@
       <c r="A109" s="5">
         <v>107</v>
       </c>
+      <c r="B109" t="s">
+        <v>25</v>
+      </c>
+      <c r="C109" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
@@ -1887,6 +1935,12 @@
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>25</v>
+      </c>
+      <c r="C111" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>